<commit_message>
Commiting after publishing package
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="-10245" yWindow="17505" windowWidth="21255" windowHeight="9450"/>
@@ -200,9 +200,6 @@
     <t>TimeEvening</t>
   </si>
   <si>
-    <t>sankaravenie5@gmail.com;sathyamoorthie5@gmail.com;sharongiftae5@gmail.com;aartiak.e5@gmail.com;sornalakshmie5@gmail.com;narenbagavathye5@gmail.com;prasanth9534@gmail.com</t>
-  </si>
-  <si>
     <t>&lt;html&gt;
 &lt;body&gt;
 &lt;p&gt;Hi Team &lt;/p&gt;&lt;/br&gt;
@@ -213,11 +210,14 @@
 &lt;/body&gt;
 &lt;/html&gt;</t>
   </si>
+  <si>
+    <t>sankaravenie5@gmail.com;sathyamoorthie5@gmail.com;sharongiftae5@gmail.com;aartiak.e5@gmail.com;sornalakshmie5@gmail.com;narenbagavathye5@gmail.com;prasanth9534@gmail.com; lakshmi.u@tiliconveli.com;naresh.kumar@e5.ai</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -605,11 +605,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -718,7 +718,7 @@
         <v>50</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -763,7 +763,7 @@
         <v>58</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1767,7 +1767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2930,7 +2930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>